<commit_message>
Add Checkout,Side Bar Menu,SmokeTest Suite
</commit_message>
<xml_diff>
--- a/Assessment_QA.xlsx
+++ b/Assessment_QA.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/navyrai_cisco_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D6D6548E-2F61-48DA-A498-FBC8E2128725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E69174A-0AFB-4022-9DC8-B26F66AD540A}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{D6D6548E-2F61-48DA-A498-FBC8E2128725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A90C596-A805-42AC-84EC-BAEBE6DEC0C2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="777" activeTab="3" xr2:uid="{67312112-DDCE-4ABD-836C-787597AADBE8}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN_MODULE " sheetId="1" r:id="rId1"/>
-    <sheet name="PRODUCT_LISTING_PAGE" sheetId="3" r:id="rId2"/>
+    <sheet name="PRODUCT_HOME_PAGE" sheetId="3" r:id="rId2"/>
     <sheet name="CRITICAL_TC_PRIORITY" sheetId="4" r:id="rId3"/>
     <sheet name="Automated Smoke Test Suite" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="393">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -1034,18 +1034,6 @@
  Test ID                      :  TC_LOGN_01</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet Name           : PRODUCT LISTING PAGE
-Test ID                      : TC_LOGN_02 </t>
-  </si>
-  <si>
-    <t>Sheet Name           : PRODUCT LISTING PAGE
- Test ID                      : TC_PRODUCT_01 to TC_PRODUCT_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheet Name           : PRODUCT LISTING PAGE
- Test ID                       : TC_ADD_CART_01 to TC_ADD_CART_03 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Filter and Sort Options - Product Name - A to Z </t>
   </si>
   <si>
@@ -1784,8 +1772,30 @@
     <t xml:space="preserve">Priority  Rank </t>
   </si>
   <si>
-    <t>Sheet Name           : PRODUCT LISTING PAGE
+    <t xml:space="preserve">Checkout Page </t>
+  </si>
+  <si>
+    <t>Ensure Check out will happen smoothly without any error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet Name           : PRODUCT HOME PAGE
+Test ID                      : TC_LOGN_02 </t>
+  </si>
+  <si>
+    <t>Sheet Name           :  : PRODUCT HOME PAGE
+ Test ID                      : TC_PRODUCT_01 to TC_PRODUCT_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet Name           :  : PRODUCT HOME PAGE
+ Test ID                       : TC_ADD_CART_01 to TC_ADD_CART_03 </t>
+  </si>
+  <si>
+    <t>Sheet Name           :  : PRODUCT HOME PAGE
 Test ID                      : TC_CART_PG_01 to TC_CART_PG_05</t>
+  </si>
+  <si>
+    <t>Sheet Name :  : PRODUCT HOME PAGE
+Test ID : TC_CHK_OT_01 to TC_CHK_OT_11</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2304,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
@@ -2342,7 +2352,7 @@
         <v>6</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -2365,30 +2375,30 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -2411,30 +2421,30 @@
         <v>54</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -2457,7 +2467,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>23</v>
@@ -2466,21 +2476,21 @@
         <v>18</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -2510,21 +2520,21 @@
         <v>22</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -2544,7 +2554,7 @@
     </row>
     <row r="15" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="12" t="s">
@@ -2554,21 +2564,21 @@
         <v>21</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -2591,30 +2601,30 @@
         <v>57</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -2637,7 +2647,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>26</v>
@@ -2646,10 +2656,10 @@
         <v>18</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>34</v>
@@ -2660,7 +2670,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -2690,21 +2700,21 @@
         <v>21</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -2734,21 +2744,21 @@
         <v>22</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -2771,7 +2781,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>29</v>
@@ -2780,10 +2790,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>43</v>
@@ -2794,7 +2804,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -2824,21 +2834,21 @@
         <v>21</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
@@ -2868,21 +2878,21 @@
         <v>22</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -2905,7 +2915,7 @@
         <v>64</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>38</v>
@@ -2914,10 +2924,10 @@
         <v>18</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>41</v>
@@ -2928,7 +2938,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -2958,21 +2968,21 @@
         <v>21</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -3002,21 +3012,21 @@
         <v>22</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -3039,7 +3049,7 @@
         <v>67</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>44</v>
@@ -3048,10 +3058,10 @@
         <v>18</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>45</v>
@@ -3062,7 +3072,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -3092,21 +3102,21 @@
         <v>21</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -3126,7 +3136,7 @@
     </row>
     <row r="28" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="12" t="s">
@@ -3136,21 +3146,21 @@
         <v>22</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>47</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -4330,7 +4340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA61B65F-699F-4680-8624-3BDF13300B44}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
@@ -4364,7 +4374,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -4439,7 +4449,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4447,7 +4457,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>23</v>
@@ -4456,19 +4466,19 @@
         <v>18</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.35">
@@ -4476,28 +4486,28 @@
         <v>54</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>35</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="102.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4505,19 +4515,19 @@
         <v>165</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>70</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>130</v>
@@ -4526,7 +4536,7 @@
         <v>71</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="104.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4534,28 +4544,28 @@
         <v>166</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.35">
@@ -4566,22 +4576,22 @@
         <v>143</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>145</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>146</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4598,19 +4608,19 @@
         <v>73</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4624,19 +4634,19 @@
         <v>75</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4650,19 +4660,19 @@
         <v>76</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>80</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="101" customHeight="1" x14ac:dyDescent="0.35">
@@ -4670,7 +4680,7 @@
         <v>171</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>81</v>
@@ -4679,19 +4689,19 @@
         <v>83</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>82</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4699,25 +4709,25 @@
         <v>172</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>85</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4725,19 +4735,19 @@
         <v>173</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>93</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>87</v>
@@ -4745,7 +4755,7 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4753,19 +4763,19 @@
         <v>174</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>88</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>94</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>91</v>
@@ -4773,7 +4783,7 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4781,19 +4791,19 @@
         <v>175</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>95</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>90</v>
@@ -4801,7 +4811,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -4824,13 +4834,13 @@
         <v>98</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>99</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -4850,13 +4860,13 @@
         <v>136</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>137</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -4876,13 +4886,13 @@
         <v>140</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>141</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4902,13 +4912,13 @@
         <v>106</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>142</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4928,13 +4938,13 @@
         <v>103</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>104</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -4954,13 +4964,13 @@
         <v>108</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>109</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="145" x14ac:dyDescent="0.35">
@@ -4968,28 +4978,28 @@
         <v>182</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D29" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>252</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4997,7 +5007,7 @@
         <v>183</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>113</v>
@@ -5006,19 +5016,19 @@
         <v>111</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>119</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>112</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -5026,7 +5036,7 @@
         <v>184</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>114</v>
@@ -5041,21 +5051,21 @@
         <v>120</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>123</v>
@@ -5070,42 +5080,42 @@
         <v>126</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>125</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H33" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>265</v>
-      </c>
       <c r="K33" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5113,7 +5123,7 @@
         <v>185</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>116</v>
@@ -5131,7 +5141,7 @@
         <v>122</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5139,28 +5149,28 @@
         <v>186</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5168,231 +5178,231 @@
         <v>187</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="H37" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="K37" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="F38" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="G38" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H38" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>276</v>
-      </c>
       <c r="K38" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="143" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E39" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>278</v>
-      </c>
       <c r="H39" s="12" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="121.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H40" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>285</v>
-      </c>
       <c r="K40" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C42" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>292</v>
-      </c>
       <c r="F42" s="12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="K42" s="12"/>
     </row>
     <row r="43" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>290</v>
-      </c>
       <c r="E43" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G43" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="K43" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>127</v>
@@ -5410,13 +5420,13 @@
         <v>129</v>
       </c>
       <c r="G44" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="K44" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -5424,13 +5434,13 @@
         <v>188</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>70</v>
@@ -5439,13 +5449,13 @@
         <v>31</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -5459,158 +5469,158 @@
         <v>131</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>132</v>
       </c>
       <c r="G46" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="K46" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="G47" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>353</v>
-      </c>
       <c r="H47" s="12" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="109" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>359</v>
-      </c>
       <c r="G48" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>365</v>
-      </c>
       <c r="E49" s="12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>366</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D51" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="G51" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>386</v>
-      </c>
       <c r="H51" s="12" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5694,10 +5704,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -5710,10 +5720,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0A56BA-8610-424D-9FDF-7E1C4B95062F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" activeCellId="1" sqref="C9 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5758,7 +5768,7 @@
         <v>160</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>192</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -5769,7 +5779,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>193</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -5780,7 +5790,7 @@
         <v>163</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>194</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -5791,7 +5801,18 @@
         <v>189</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>